<commit_message>
Changed data and files
</commit_message>
<xml_diff>
--- a/Data/Agricultural_use.xlsx
+++ b/Data/Agricultural_use.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charly\Documents\Data Science\Projects\water_management\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBEEAB8-2190-4395-9058-BCE5C549493E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCA5F768-1FF3-41D2-906A-C03078B2CD14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7935" yWindow="4575" windowWidth="27960" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2235" yWindow="3825" windowWidth="27960" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,6 @@
     <t>Clave</t>
   </si>
   <si>
-    <t xml:space="preserve">Nombre </t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>Aguas del Valle de México</t>
+  </si>
+  <si>
+    <t>Nombre</t>
   </si>
 </sst>
 </file>
@@ -482,7 +482,7 @@
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q19" sqref="Q19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +496,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1">
         <v>2005</v>
@@ -546,10 +546,10 @@
     </row>
     <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="C2" s="3">
         <v>5248.11</v>
@@ -599,10 +599,10 @@
     </row>
     <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="C3" s="3">
         <v>11153.63</v>
@@ -652,10 +652,10 @@
     </row>
     <row r="4" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="C4" s="3">
         <v>18537.509999999998</v>
@@ -705,10 +705,10 @@
     </row>
     <row r="5" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C5" s="3">
         <v>11734.63</v>
@@ -758,10 +758,10 @@
     </row>
     <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C6" s="3">
         <v>1900.88</v>
@@ -811,10 +811,10 @@
     </row>
     <row r="7" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C7" s="3">
         <v>14659.57</v>
@@ -864,10 +864,10 @@
     </row>
     <row r="8" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
       </c>
       <c r="C8" s="3">
         <v>6297.48</v>
@@ -917,10 +917,10 @@
     </row>
     <row r="9" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="C9" s="3">
         <v>20320.47</v>
@@ -970,10 +970,10 @@
     </row>
     <row r="10" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="C10" s="3">
         <v>6362.66</v>
@@ -1023,10 +1023,10 @@
     </row>
     <row r="11" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="C11" s="3">
         <v>3923.02</v>
@@ -1076,10 +1076,10 @@
     </row>
     <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="C12" s="3">
         <v>2867.43</v>
@@ -1129,10 +1129,10 @@
     </row>
     <row r="13" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="C13" s="3">
         <v>1614.8</v>
@@ -1182,10 +1182,10 @@
     </row>
     <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="C14" s="3">
         <v>4201.41</v>

</xml_diff>